<commit_message>
ceta serah terim bn dp5nt38
</commit_message>
<xml_diff>
--- a/15. DP 4N32 (F4 MERAH)/NAME TAG.xlsx
+++ b/15. DP 4N32 (F4 MERAH)/NAME TAG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\15. DP 4N32 (F4 MERAH)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3467A97-9441-4340-8F62-4B7C7EB10568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{77F2A49D-8265-4467-B84D-619F17078A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -20,14 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+  <si>
+    <t>NO</t>
+  </si>
   <si>
     <t>AGUS SUTANTO</t>
   </si>
   <si>
-    <t>MOH.TAUFIK</t>
-  </si>
-  <si>
     <t xml:space="preserve">EDI PURWANTO </t>
   </si>
   <si>
@@ -40,50 +40,65 @@
     <t>TOTOK ELFIANTO</t>
   </si>
   <si>
-    <t>M.ARIFAI</t>
-  </si>
-  <si>
-    <t>M.MUSTOFA</t>
-  </si>
-  <si>
-    <t>NO</t>
+    <t>EKO HADI P</t>
+  </si>
+  <si>
+    <t>FAISHAL ARIEF</t>
+  </si>
+  <si>
+    <t>ROBI JARKASIH</t>
+  </si>
+  <si>
+    <t>SAIFUL ARIFIN</t>
   </si>
   <si>
     <t xml:space="preserve">VIRGO HANDOYO </t>
   </si>
   <si>
-    <t>FAISHAL ARIEF</t>
-  </si>
-  <si>
-    <t>ROBI JARKASIH</t>
-  </si>
-  <si>
-    <t>KHISBULLAHHUDA</t>
-  </si>
-  <si>
-    <t>EKO HADI P</t>
-  </si>
-  <si>
-    <t>SAIFUL ARIFIN</t>
-  </si>
-  <si>
-    <t>DP 4 NAUTIKA ANGK. 32</t>
+    <t>KHISBULLAH HUDA</t>
+  </si>
+  <si>
+    <t>M. ARIFAI</t>
+  </si>
+  <si>
+    <t>M. MUSTOFA</t>
+  </si>
+  <si>
+    <t>MOH. TAUFIK</t>
+  </si>
+  <si>
+    <t>MUHAMMAD KHOLIF</t>
+  </si>
+  <si>
+    <t>NAMA</t>
   </si>
   <si>
     <t>KELAS</t>
   </si>
   <si>
-    <t>NAMA</t>
-  </si>
-  <si>
-    <t>MUHAMMAD KHOLIF</t>
+    <t>DP 4 NAUTIKA/32</t>
+  </si>
+  <si>
+    <t>NOVAN SURYO S.</t>
+  </si>
+  <si>
+    <t>WARSONO</t>
+  </si>
+  <si>
+    <t>ACHMAD SUBANDRIYO</t>
+  </si>
+  <si>
+    <t>YAFETH B.</t>
+  </si>
+  <si>
+    <t>M. HASIM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,14 +234,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -584,22 +605,31 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -956,209 +986,257 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A5" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="4.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="B9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="B10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="B11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="C12" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C13" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="B14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="C14" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
       <c r="B16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B18">
+    <sortCondition ref="B2:B18"/>
+  </sortState>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>